<commit_message>
Mise à jour de la génération des rapports  ajoute de resume rapport
Mise à jour de la génération des rapports  ajoute de resume rapport
</commit_message>
<xml_diff>
--- a/apps/Exemple_rapport_thermique/resume_rapport_thermique_exemple.xlsx
+++ b/apps/Exemple_rapport_thermique/resume_rapport_thermique_exemple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAMER\Documents\Projects\vocasara4\Vocasar4\vocasara_webapp_update\Vocasara-full-app\Webapp - final version (correct) - Copie\Exemple_rapport_thermique\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAMER\Desktop\VocaSaraAppV2\apps\Exemple_rapport_thermique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAE95B1-B380-4A82-B9BC-58AF900B965F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA28DE03-8224-474D-ABC6-98E012EBFE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -75,6 +75,9 @@
     <t>Localisations</t>
   </si>
   <si>
+    <t xml:space="preserve">Defauts visibles </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Urgences</t>
   </si>
   <si>
@@ -96,6 +99,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t xml:space="preserve">RESUME DES RAPPORTS DE VISITE D' OUVRAGES </t>
+  </si>
+  <si>
     <t>Noms des images</t>
   </si>
   <si>
@@ -105,13 +111,7 @@
     <t>Nom :</t>
   </si>
   <si>
-    <t xml:space="preserve">Defauts insibles </t>
-  </si>
-  <si>
-    <t>Température_defaut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESUME DES RAPPORTS DE VISITE D' OUVRAGES (THERMIQUE) </t>
+    <t>Temperatures</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -533,22 +533,20 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -557,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -615,10 +613,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -651,13 +645,17 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -731,7 +729,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -742,12 +740,27 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -772,14 +785,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="medium">
           <color indexed="64"/>
         </top>
@@ -1113,7 +1124,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center"/>
       <border outline="0">
         <left/>
@@ -1272,9 +1283,9 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="troncons" dataDxfId="9"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="longueurs" dataDxfId="8"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Noms des images" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{343BC70F-7AC0-4060-9C80-6E64D69A7E7A}" name="Température_defaut" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Localisations" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Defauts insibles " dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Defauts visibles " dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{40DEBFB9-CB30-4B23-83BD-D6B02A113A5F}" name="Temperatures" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name=" Urgences" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="conseils" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="normes" dataDxfId="2"/>
@@ -1583,28 +1594,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" style="28" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" style="28" customWidth="1"/>
-    <col min="5" max="6" width="81.140625" style="28" customWidth="1"/>
-    <col min="7" max="7" width="80.5703125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="110.42578125" style="28" customWidth="1"/>
-    <col min="9" max="9" width="39.7109375" style="28" customWidth="1"/>
-    <col min="10" max="10" width="120.42578125" style="28" customWidth="1"/>
-    <col min="11" max="11" width="119.85546875" style="28" customWidth="1"/>
-    <col min="12" max="12" width="24.42578125" style="28" customWidth="1"/>
-    <col min="13" max="14" width="10.85546875" style="28" customWidth="1"/>
-    <col min="15" max="16384" width="10.85546875" style="28"/>
+    <col min="1" max="1" width="43" style="27" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="81.140625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="80.5703125" style="27" customWidth="1"/>
+    <col min="7" max="7" width="110.42578125" style="27" customWidth="1"/>
+    <col min="8" max="8" width="71.28515625" style="27" customWidth="1"/>
+    <col min="9" max="9" width="39.7109375" style="27" customWidth="1"/>
+    <col min="10" max="10" width="120.42578125" style="27" customWidth="1"/>
+    <col min="11" max="11" width="119.85546875" style="27" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" style="27" customWidth="1"/>
+    <col min="13" max="14" width="10.85546875" style="27" customWidth="1"/>
+    <col min="15" max="16384" width="10.85546875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="19" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="18" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48"/>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -1618,9 +1630,9 @@
       <c r="K1" s="49"/>
       <c r="L1" s="49"/>
     </row>
-    <row r="2" spans="1:12" s="20" customFormat="1" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="19" customFormat="1" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1634,7 +1646,7 @@
       <c r="K2" s="39"/>
       <c r="L2" s="47"/>
     </row>
-    <row r="3" spans="1:12" s="19" customFormat="1" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="18" customFormat="1" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>0</v>
       </c>
@@ -1642,33 +1654,33 @@
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="37"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="42"/>
+      <c r="F3" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="58"/>
       <c r="I3" s="44" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="45"/>
       <c r="K3" s="45"/>
       <c r="L3" s="46"/>
     </row>
-    <row r="4" spans="1:12" s="19" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="18" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40"/>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
       <c r="E4" s="41"/>
-      <c r="F4" s="31"/>
+      <c r="F4" s="43"/>
       <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="H4" s="29"/>
       <c r="I4" s="38"/>
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
       <c r="L4" s="47"/>
     </row>
-    <row r="5" spans="1:12" s="19" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="18" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
@@ -1676,14 +1688,14 @@
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="50" t="s">
+      <c r="F5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="57">
+      <c r="H5" s="62"/>
+      <c r="I5" s="61">
         <v>0</v>
       </c>
       <c r="J5" s="56" t="s">
@@ -1692,31 +1704,31 @@
       <c r="K5" s="33"/>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="1:12" s="19" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="18" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38"/>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
       <c r="E6" s="39"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="50" t="s">
-        <v>22</v>
-      </c>
+      <c r="F6" s="51"/>
+      <c r="G6" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="59"/>
       <c r="I6" s="55"/>
       <c r="J6" s="34"/>
       <c r="K6" s="35"/>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:12" s="19" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="18" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="40"/>
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
       <c r="E7" s="41"/>
-      <c r="F7" s="31"/>
+      <c r="F7" s="43"/>
       <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="54">
         <v>1</v>
       </c>
@@ -1726,36 +1738,36 @@
       <c r="K7" s="33"/>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" s="19" customFormat="1" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="18" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
-      <c r="F8" s="30"/>
+      <c r="F8" s="50" t="s">
+        <v>6</v>
+      </c>
       <c r="G8" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H8" s="59"/>
       <c r="I8" s="55"/>
       <c r="J8" s="34"/>
       <c r="K8" s="35"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" s="19" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
-      <c r="F9" s="29"/>
+      <c r="F9" s="51"/>
       <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="58">
+      <c r="H9" s="31"/>
+      <c r="I9" s="57">
         <v>2</v>
       </c>
       <c r="J9" s="52" t="s">
@@ -1764,67 +1776,67 @@
       <c r="K9" s="33"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" s="19" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="18" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="40"/>
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
       <c r="E10" s="41"/>
-      <c r="F10" s="31"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
+      <c r="H10" s="28"/>
       <c r="I10" s="43"/>
       <c r="J10" s="40"/>
       <c r="K10" s="41"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:12" s="19" customFormat="1" ht="42.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:12" s="18" customFormat="1" ht="42.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>24</v>
+      <c r="E11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="H11" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="J11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="K11" s="21" t="s">
         <v>16</v>
       </c>
+      <c r="L11" s="26" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" s="19" customFormat="1" ht="130.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="18" customFormat="1" ht="130.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="8"/>
       <c r="D12" s="3"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="6"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="60"/>
       <c r="I12" s="15"/>
       <c r="J12" s="16"/>
       <c r="K12" s="17"/>
@@ -1836,19 +1848,19 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J7:K8"/>
     <mergeCell ref="A5:E7"/>
-    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="I3:L4"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A8:E10"/>
-    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F8:F10"/>
     <mergeCell ref="J9:K10"/>
     <mergeCell ref="A2:L2"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J5:K6"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G8:G10"/>
     <mergeCell ref="A3:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>